<commit_message>
reformating parameters files and db
</commit_message>
<xml_diff>
--- a/input/params_main.xlsx
+++ b/input/params_main.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21300" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">parameters!$A$1:$F$550</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">parameters!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3085" uniqueCount="680">
   <si>
     <t>emi_master</t>
   </si>
@@ -2047,6 +2047,21 @@
   </si>
   <si>
     <t>tbd</t>
+  </si>
+  <si>
+    <t>PP_CM_IPT_H</t>
+  </si>
+  <si>
+    <t>COMP_AVG_HARDNESS</t>
+  </si>
+  <si>
+    <t>COAT_AVG_HARDNESS</t>
+  </si>
+  <si>
+    <t>range_min</t>
+  </si>
+  <si>
+    <t>range_max</t>
   </si>
 </sst>
 </file>
@@ -2088,7 +2103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2101,6 +2116,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2471,11 +2489,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F550"/>
+  <dimension ref="A1:H566"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A545" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,10 +2504,12 @@
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="35.5703125" customWidth="1"/>
     <col min="6" max="6" width="19.140625" style="2" customWidth="1"/>
-    <col min="7" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2508,8 +2528,14 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>678</v>
+      </c>
+      <c r="H1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -2529,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2549,7 +2575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2569,7 +2595,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2589,7 +2615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2609,7 +2635,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2629,7 +2655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2649,7 +2675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -2669,7 +2695,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2689,7 +2715,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2709,7 +2735,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -2729,7 +2755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>29</v>
       </c>
@@ -2749,7 +2775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -2769,7 +2795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -2789,7 +2815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -13489,8 +13515,310 @@
         <v>2</v>
       </c>
     </row>
+    <row r="551" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A551" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B551" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C551" t="s">
+        <v>108</v>
+      </c>
+      <c r="D551" t="s">
+        <v>42</v>
+      </c>
+      <c r="E551" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F551" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="552" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A552" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B552" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C552" t="s">
+        <v>108</v>
+      </c>
+      <c r="D552" t="s">
+        <v>42</v>
+      </c>
+      <c r="E552" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F552" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="553" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A553" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B553" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C553" t="s">
+        <v>108</v>
+      </c>
+      <c r="D553" t="s">
+        <v>42</v>
+      </c>
+      <c r="E553" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F553" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="554" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A554" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B554" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C554" t="s">
+        <v>557</v>
+      </c>
+      <c r="D554" t="s">
+        <v>42</v>
+      </c>
+      <c r="E554" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F554" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A555" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B555" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C555" t="s">
+        <v>557</v>
+      </c>
+      <c r="D555" t="s">
+        <v>42</v>
+      </c>
+      <c r="E555" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F555" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="556" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A556" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B556" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C556" t="s">
+        <v>557</v>
+      </c>
+      <c r="D556" t="s">
+        <v>42</v>
+      </c>
+      <c r="E556" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F556" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="557" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A557" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B557" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C557" t="s">
+        <v>557</v>
+      </c>
+      <c r="D557" t="s">
+        <v>559</v>
+      </c>
+      <c r="E557" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="F557" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="558" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A558" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B558" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C558" t="s">
+        <v>156</v>
+      </c>
+      <c r="D558" t="s">
+        <v>42</v>
+      </c>
+      <c r="E558" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F558" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="559" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A559" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B559" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C559" t="s">
+        <v>156</v>
+      </c>
+      <c r="D559" t="s">
+        <v>42</v>
+      </c>
+      <c r="E559" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F559" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="560" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A560" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B560" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C560" t="s">
+        <v>156</v>
+      </c>
+      <c r="D560" t="s">
+        <v>42</v>
+      </c>
+      <c r="E560" s="7" t="s">
+        <v>676</v>
+      </c>
+      <c r="F560" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="561" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A561" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B561" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C561" t="s">
+        <v>108</v>
+      </c>
+      <c r="D561" t="s">
+        <v>42</v>
+      </c>
+      <c r="F561" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="562" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A562" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B562" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C562" t="s">
+        <v>108</v>
+      </c>
+      <c r="D562" t="s">
+        <v>42</v>
+      </c>
+      <c r="F562" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="563" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A563" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B563" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="C563" t="s">
+        <v>108</v>
+      </c>
+      <c r="D563" t="s">
+        <v>42</v>
+      </c>
+      <c r="F563" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="564" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A564" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C564" t="s">
+        <v>108</v>
+      </c>
+      <c r="D564" t="s">
+        <v>42</v>
+      </c>
+      <c r="F564" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="565" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A565" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B565" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C565" t="s">
+        <v>108</v>
+      </c>
+      <c r="D565" t="s">
+        <v>42</v>
+      </c>
+      <c r="F565" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="566" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A566" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B566" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C566" t="s">
+        <v>108</v>
+      </c>
+      <c r="D566" t="s">
+        <v>42</v>
+      </c>
+      <c r="F566" s="2">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F550"/>
+  <autoFilter ref="A1:H1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Removed duplicated parameter COMP_MEAN_WEIGHT
</commit_message>
<xml_diff>
--- a/input/params_main.xlsx
+++ b/input/params_main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sobczakk\OneDrive - Takeda\Documents\GIT REPOS\cpv\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_175EAAC150BB7296499C3516F21ABD484EA7ED2B" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{0E2F965E-473B-40FD-BFF6-807464D6179C}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_175EAAC150BB7296499C3516F21ABD484EA7ED2B" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{B2E17C8E-E193-4023-BED0-9C8B41574384}"/>
   <bookViews>
-    <workbookView xWindow="31215" yWindow="1515" windowWidth="26385" windowHeight="14415" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="465" windowWidth="21315" windowHeight="12165" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
@@ -2359,7 +2359,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E325" sqref="E325:E357"/>
+      <selection pane="bottomLeft" activeCell="B341" sqref="B341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
No ranges file added, new CF parameters
</commit_message>
<xml_diff>
--- a/input/params_main.xlsx
+++ b/input/params_main.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sobczakk\OneDrive - Takeda\Documents\GIT REPOS\cpv\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sobczakk\Documents\GIT REPOS\cpv\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="11_175EAAC150BB7296499C3516F21ABD484EA7ED2B" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{C6C5B48E-2AB0-4B92-A879-A1341D3F903E}"/>
   <bookViews>
-    <workbookView xWindow="7065" yWindow="930" windowWidth="21600" windowHeight="14550" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7065" yWindow="930" windowWidth="21600" windowHeight="14550" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="parameters" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">parameters!$A$1:$F$505</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">parameters!$A$1:$F$537</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2953" uniqueCount="776">
   <si>
     <t>emi_master</t>
   </si>
@@ -2224,12 +2223,150 @@
   </si>
   <si>
     <t>ECM_YIELD</t>
+  </si>
+  <si>
+    <t>TIL_FIRSTDRUM_PSDT7</t>
+  </si>
+  <si>
+    <t>TIL_FIRSTDRUM_PSDT8</t>
+  </si>
+  <si>
+    <t>TIL_FIRSTDRUM_RESULT27</t>
+  </si>
+  <si>
+    <t>TIL_FIRSTDRUM_RESULT28</t>
+  </si>
+  <si>
+    <t>TIL_IPT_ERH_%7</t>
+  </si>
+  <si>
+    <t>TIL_IPT_ERH_%8</t>
+  </si>
+  <si>
+    <t>TIL_CF_SPRAY_QTY_LOT1</t>
+  </si>
+  <si>
+    <t>TIL_CF_SPRAY_QTY_LOT2</t>
+  </si>
+  <si>
+    <t>TIL_CF_SPRAY_QTY_LOT3</t>
+  </si>
+  <si>
+    <t>TIL_CF_SPRAY_QTY_LOT4</t>
+  </si>
+  <si>
+    <t>TIL_CF_SPRAY_QTY_LOT5</t>
+  </si>
+  <si>
+    <t>TIL_CF_SPRAY_QTY_LOT6</t>
+  </si>
+  <si>
+    <t>TIL_CF_SPRAY_QTY_LOT7</t>
+  </si>
+  <si>
+    <t>TIL_CF_SPRAY_QTY_LOT8</t>
+  </si>
+  <si>
+    <t>PSD1</t>
+  </si>
+  <si>
+    <t>PSD2</t>
+  </si>
+  <si>
+    <t>PSD3</t>
+  </si>
+  <si>
+    <t>PSD4</t>
+  </si>
+  <si>
+    <t>PSD5</t>
+  </si>
+  <si>
+    <t>PSD6</t>
+  </si>
+  <si>
+    <t>PSD7</t>
+  </si>
+  <si>
+    <t>PSD8</t>
+  </si>
+  <si>
+    <t>SV1</t>
+  </si>
+  <si>
+    <t>SV2</t>
+  </si>
+  <si>
+    <t>SV3</t>
+  </si>
+  <si>
+    <t>SV4</t>
+  </si>
+  <si>
+    <t>SV5</t>
+  </si>
+  <si>
+    <t>SV6</t>
+  </si>
+  <si>
+    <t>SV7</t>
+  </si>
+  <si>
+    <t>SV8</t>
+  </si>
+  <si>
+    <t>ERH1</t>
+  </si>
+  <si>
+    <t>ERH2</t>
+  </si>
+  <si>
+    <t>ERH3</t>
+  </si>
+  <si>
+    <t>ERH4</t>
+  </si>
+  <si>
+    <t>ERH5</t>
+  </si>
+  <si>
+    <t>ERH6</t>
+  </si>
+  <si>
+    <t>ERH7</t>
+  </si>
+  <si>
+    <t>ERH8</t>
+  </si>
+  <si>
+    <t>Totalspratamt1</t>
+  </si>
+  <si>
+    <t>Totalspratamt2</t>
+  </si>
+  <si>
+    <t>Totalspratamt3</t>
+  </si>
+  <si>
+    <t>Totalspratamt4</t>
+  </si>
+  <si>
+    <t>Totalspratamt5</t>
+  </si>
+  <si>
+    <t>Totalspratamt6</t>
+  </si>
+  <si>
+    <t>Totalspratamt7</t>
+  </si>
+  <si>
+    <t>Totalspratamt8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2441,23 +2578,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2493,23 +2613,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2685,12 +2788,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F505"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F537"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E523" sqref="E523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12805,14 +12908,654 @@
         <v>543</v>
       </c>
     </row>
+    <row r="506" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A506" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B506" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C506" t="s">
+        <v>215</v>
+      </c>
+      <c r="D506" t="s">
+        <v>216</v>
+      </c>
+      <c r="E506" t="s">
+        <v>744</v>
+      </c>
+      <c r="F506" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="507" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A507" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B507" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C507" t="s">
+        <v>215</v>
+      </c>
+      <c r="D507" t="s">
+        <v>216</v>
+      </c>
+      <c r="E507" t="s">
+        <v>745</v>
+      </c>
+      <c r="F507" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="508" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A508" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B508" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C508" t="s">
+        <v>215</v>
+      </c>
+      <c r="D508" t="s">
+        <v>216</v>
+      </c>
+      <c r="E508" t="s">
+        <v>746</v>
+      </c>
+      <c r="F508" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="509" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A509" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B509" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C509" t="s">
+        <v>215</v>
+      </c>
+      <c r="D509" t="s">
+        <v>216</v>
+      </c>
+      <c r="E509" t="s">
+        <v>747</v>
+      </c>
+      <c r="F509" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="510" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A510" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B510" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C510" t="s">
+        <v>215</v>
+      </c>
+      <c r="D510" t="s">
+        <v>216</v>
+      </c>
+      <c r="E510" t="s">
+        <v>748</v>
+      </c>
+      <c r="F510" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="511" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A511" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B511" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C511" t="s">
+        <v>215</v>
+      </c>
+      <c r="D511" t="s">
+        <v>216</v>
+      </c>
+      <c r="E511" t="s">
+        <v>749</v>
+      </c>
+      <c r="F511" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="512" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A512" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B512" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="C512" t="s">
+        <v>215</v>
+      </c>
+      <c r="D512" t="s">
+        <v>216</v>
+      </c>
+      <c r="E512" t="s">
+        <v>750</v>
+      </c>
+      <c r="F512" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="513" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A513" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B513" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="C513" t="s">
+        <v>215</v>
+      </c>
+      <c r="D513" t="s">
+        <v>216</v>
+      </c>
+      <c r="E513" t="s">
+        <v>751</v>
+      </c>
+      <c r="F513" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="514" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A514" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B514" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C514" t="s">
+        <v>215</v>
+      </c>
+      <c r="D514" t="s">
+        <v>216</v>
+      </c>
+      <c r="E514" t="s">
+        <v>752</v>
+      </c>
+      <c r="F514" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="515" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A515" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B515" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C515" t="s">
+        <v>215</v>
+      </c>
+      <c r="D515" t="s">
+        <v>216</v>
+      </c>
+      <c r="E515" t="s">
+        <v>753</v>
+      </c>
+      <c r="F515" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="516" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A516" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B516" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C516" t="s">
+        <v>215</v>
+      </c>
+      <c r="D516" t="s">
+        <v>216</v>
+      </c>
+      <c r="E516" t="s">
+        <v>754</v>
+      </c>
+      <c r="F516" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="517" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A517" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B517" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C517" t="s">
+        <v>215</v>
+      </c>
+      <c r="D517" t="s">
+        <v>216</v>
+      </c>
+      <c r="E517" t="s">
+        <v>755</v>
+      </c>
+      <c r="F517" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="518" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A518" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B518" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C518" t="s">
+        <v>215</v>
+      </c>
+      <c r="D518" t="s">
+        <v>216</v>
+      </c>
+      <c r="E518" t="s">
+        <v>756</v>
+      </c>
+      <c r="F518" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A519" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B519" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C519" t="s">
+        <v>215</v>
+      </c>
+      <c r="D519" t="s">
+        <v>216</v>
+      </c>
+      <c r="E519" t="s">
+        <v>757</v>
+      </c>
+      <c r="F519" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="520" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A520" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B520" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="C520" t="s">
+        <v>215</v>
+      </c>
+      <c r="D520" t="s">
+        <v>216</v>
+      </c>
+      <c r="E520" t="s">
+        <v>758</v>
+      </c>
+      <c r="F520" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="521" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A521" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B521" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="C521" t="s">
+        <v>215</v>
+      </c>
+      <c r="D521" t="s">
+        <v>216</v>
+      </c>
+      <c r="E521" t="s">
+        <v>759</v>
+      </c>
+      <c r="F521" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="522" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A522" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B522" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C522" t="s">
+        <v>215</v>
+      </c>
+      <c r="D522" t="s">
+        <v>216</v>
+      </c>
+      <c r="E522" t="s">
+        <v>760</v>
+      </c>
+      <c r="F522" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="523" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A523" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B523" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C523" t="s">
+        <v>215</v>
+      </c>
+      <c r="D523" t="s">
+        <v>216</v>
+      </c>
+      <c r="E523" t="s">
+        <v>761</v>
+      </c>
+      <c r="F523" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="524" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A524" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B524" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C524" t="s">
+        <v>215</v>
+      </c>
+      <c r="D524" t="s">
+        <v>216</v>
+      </c>
+      <c r="E524" t="s">
+        <v>762</v>
+      </c>
+      <c r="F524" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="525" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A525" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B525" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C525" t="s">
+        <v>215</v>
+      </c>
+      <c r="D525" t="s">
+        <v>216</v>
+      </c>
+      <c r="E525" t="s">
+        <v>763</v>
+      </c>
+      <c r="F525" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="526" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A526" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B526" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C526" t="s">
+        <v>215</v>
+      </c>
+      <c r="D526" t="s">
+        <v>216</v>
+      </c>
+      <c r="E526" t="s">
+        <v>764</v>
+      </c>
+      <c r="F526" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="527" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A527" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B527" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C527" t="s">
+        <v>215</v>
+      </c>
+      <c r="D527" t="s">
+        <v>216</v>
+      </c>
+      <c r="E527" t="s">
+        <v>765</v>
+      </c>
+      <c r="F527" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="528" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A528" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B528" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="C528" t="s">
+        <v>215</v>
+      </c>
+      <c r="D528" t="s">
+        <v>216</v>
+      </c>
+      <c r="E528" t="s">
+        <v>766</v>
+      </c>
+      <c r="F528" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="529" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A529" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B529" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="C529" t="s">
+        <v>215</v>
+      </c>
+      <c r="D529" t="s">
+        <v>216</v>
+      </c>
+      <c r="E529" t="s">
+        <v>767</v>
+      </c>
+      <c r="F529" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="530" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A530" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B530" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="C530" t="s">
+        <v>215</v>
+      </c>
+      <c r="D530" t="s">
+        <v>216</v>
+      </c>
+      <c r="E530" t="s">
+        <v>768</v>
+      </c>
+      <c r="F530" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="531" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A531" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B531" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="C531" t="s">
+        <v>215</v>
+      </c>
+      <c r="D531" t="s">
+        <v>216</v>
+      </c>
+      <c r="E531" t="s">
+        <v>769</v>
+      </c>
+      <c r="F531" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="532" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A532" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B532" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="C532" t="s">
+        <v>215</v>
+      </c>
+      <c r="D532" t="s">
+        <v>216</v>
+      </c>
+      <c r="E532" t="s">
+        <v>770</v>
+      </c>
+      <c r="F532" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="533" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A533" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B533" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="C533" t="s">
+        <v>215</v>
+      </c>
+      <c r="D533" t="s">
+        <v>216</v>
+      </c>
+      <c r="E533" t="s">
+        <v>771</v>
+      </c>
+      <c r="F533" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="534" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A534" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B534" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="C534" t="s">
+        <v>215</v>
+      </c>
+      <c r="D534" t="s">
+        <v>216</v>
+      </c>
+      <c r="E534" t="s">
+        <v>772</v>
+      </c>
+      <c r="F534" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="535" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A535" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B535" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="C535" t="s">
+        <v>215</v>
+      </c>
+      <c r="D535" t="s">
+        <v>216</v>
+      </c>
+      <c r="E535" t="s">
+        <v>773</v>
+      </c>
+      <c r="F535" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="536" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A536" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B536" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="C536" t="s">
+        <v>215</v>
+      </c>
+      <c r="D536" t="s">
+        <v>216</v>
+      </c>
+      <c r="E536" t="s">
+        <v>774</v>
+      </c>
+      <c r="F536" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="537" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A537" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B537" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="C537" t="s">
+        <v>215</v>
+      </c>
+      <c r="D537" t="s">
+        <v>216</v>
+      </c>
+      <c r="E537" t="s">
+        <v>775</v>
+      </c>
+      <c r="F537" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F505" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F505">
+  <autoFilter ref="A1:F537">
+    <sortState ref="A2:F505">
       <sortCondition ref="A2:A505"/>
       <sortCondition ref="B2:B505"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H538">
+  <sortState ref="A2:H538">
     <sortCondition ref="A2:A538"/>
     <sortCondition ref="D2:D538"/>
     <sortCondition ref="B2:B538"/>

</xml_diff>